<commit_message>
clean up, "Cohorts.csv" removed from function, excludednodes turned into parameter in the SQL file
</commit_message>
<xml_diff>
--- a/PhenChange.xlsx
+++ b/PhenChange.xlsx
@@ -11617,13 +11617,13 @@
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>12824</v>
+        <v>12822</v>
       </c>
       <c r="B132" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C132" t="s">
-        <v>87</v>
+        <v>184</v>
       </c>
       <c r="D132" t="n">
         <v>0</v>
@@ -11693,13 +11693,13 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>12822</v>
+        <v>12824</v>
       </c>
       <c r="B134" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C134" t="s">
-        <v>184</v>
+        <v>87</v>
       </c>
       <c r="D134" t="n">
         <v>0</v>
@@ -17393,13 +17393,13 @@
     </row>
     <row r="284">
       <c r="A284" t="n">
-        <v>12824</v>
+        <v>12822</v>
       </c>
       <c r="B284" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C284" t="s">
-        <v>87</v>
+        <v>184</v>
       </c>
       <c r="D284" t="n">
         <v>0</v>
@@ -17469,13 +17469,13 @@
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>12822</v>
+        <v>12824</v>
       </c>
       <c r="B286" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C286" t="s">
-        <v>184</v>
+        <v>87</v>
       </c>
       <c r="D286" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
renamed package, make it use temp tables
</commit_message>
<xml_diff>
--- a/PhenChange.xlsx
+++ b/PhenChange.xlsx
@@ -12453,13 +12453,13 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>12822</v>
+        <v>12824</v>
       </c>
       <c r="B154" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C154" t="s">
-        <v>184</v>
+        <v>87</v>
       </c>
       <c r="D154" t="n">
         <v>0</v>
@@ -12529,13 +12529,13 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>12824</v>
+        <v>12822</v>
       </c>
       <c r="B156" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C156" t="s">
-        <v>87</v>
+        <v>184</v>
       </c>
       <c r="D156" t="n">
         <v>0</v>
@@ -13669,13 +13669,13 @@
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>12822</v>
+        <v>12825</v>
       </c>
       <c r="B186" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C186" t="s">
-        <v>362</v>
+        <v>78</v>
       </c>
       <c r="D186" t="n">
         <v>0</v>
@@ -13684,10 +13684,10 @@
         <v>1</v>
       </c>
       <c r="F186" t="n">
-        <v>439147</v>
+        <v>443432</v>
       </c>
       <c r="G186" t="s">
-        <v>362</v>
+        <v>79</v>
       </c>
       <c r="H186" t="s">
         <v>3</v>
@@ -13745,13 +13745,13 @@
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>12825</v>
+        <v>12822</v>
       </c>
       <c r="B188" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C188" t="s">
-        <v>78</v>
+        <v>362</v>
       </c>
       <c r="D188" t="n">
         <v>0</v>
@@ -13760,10 +13760,10 @@
         <v>1</v>
       </c>
       <c r="F188" t="n">
-        <v>443432</v>
+        <v>439147</v>
       </c>
       <c r="G188" t="s">
-        <v>79</v>
+        <v>362</v>
       </c>
       <c r="H188" t="s">
         <v>3</v>
@@ -17393,13 +17393,13 @@
     </row>
     <row r="284">
       <c r="A284" t="n">
-        <v>12822</v>
+        <v>12824</v>
       </c>
       <c r="B284" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C284" t="s">
-        <v>184</v>
+        <v>87</v>
       </c>
       <c r="D284" t="n">
         <v>0</v>
@@ -17469,13 +17469,13 @@
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>12824</v>
+        <v>12822</v>
       </c>
       <c r="B286" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C286" t="s">
-        <v>87</v>
+        <v>184</v>
       </c>
       <c r="D286" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
clean up, working on documentation
</commit_message>
<xml_diff>
--- a/PhenChange.xlsx
+++ b/PhenChange.xlsx
@@ -90,7 +90,7 @@
     <t xml:space="preserve">SOURCE_CONCEPT_ID</t>
   </si>
   <si>
-    <t xml:space="preserve">TOTALCOUNT</t>
+    <t xml:space="preserve">sourceCodesCount</t>
   </si>
   <si>
     <t xml:space="preserve">ACTION</t>
@@ -1104,13 +1104,13 @@
     <t xml:space="preserve">OMOP5166184</t>
   </si>
   <si>
+    <t xml:space="preserve">Exacerbation of amnesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OMOP5165900</t>
+  </si>
+  <si>
     <t xml:space="preserve">Amnesia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exacerbation of amnesia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OMOP5165900</t>
   </si>
   <si>
     <t xml:space="preserve">O/E - salaam attack</t>
@@ -11617,13 +11617,13 @@
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>12822</v>
+        <v>12824</v>
       </c>
       <c r="B132" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C132" t="s">
-        <v>184</v>
+        <v>87</v>
       </c>
       <c r="D132" t="n">
         <v>0</v>
@@ -11693,13 +11693,13 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>12824</v>
+        <v>12822</v>
       </c>
       <c r="B134" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C134" t="s">
-        <v>87</v>
+        <v>184</v>
       </c>
       <c r="D134" t="n">
         <v>0</v>
@@ -12453,13 +12453,13 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>12822</v>
+        <v>12824</v>
       </c>
       <c r="B154" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C154" t="s">
-        <v>184</v>
+        <v>87</v>
       </c>
       <c r="D154" t="n">
         <v>0</v>
@@ -12529,13 +12529,13 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>12824</v>
+        <v>12822</v>
       </c>
       <c r="B156" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C156" t="s">
-        <v>87</v>
+        <v>184</v>
       </c>
       <c r="D156" t="n">
         <v>0</v>
@@ -13441,13 +13441,13 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>12825</v>
+        <v>12822</v>
       </c>
       <c r="B180" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C180" t="s">
-        <v>362</v>
+        <v>78</v>
       </c>
       <c r="D180" t="n">
         <v>0</v>
@@ -13456,10 +13456,10 @@
         <v>1</v>
       </c>
       <c r="F180" t="n">
-        <v>439147</v>
+        <v>443432</v>
       </c>
       <c r="G180" t="s">
-        <v>362</v>
+        <v>79</v>
       </c>
       <c r="H180" t="s">
         <v>3</v>
@@ -13468,10 +13468,10 @@
         <v>1340245</v>
       </c>
       <c r="J180" t="s">
+        <v>362</v>
+      </c>
+      <c r="K180" t="s">
         <v>363</v>
-      </c>
-      <c r="K180" t="s">
-        <v>364</v>
       </c>
       <c r="L180" t="n">
         <v>0</v>
@@ -13517,13 +13517,13 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>12822</v>
+        <v>12825</v>
       </c>
       <c r="B182" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C182" t="s">
-        <v>78</v>
+        <v>364</v>
       </c>
       <c r="D182" t="n">
         <v>0</v>
@@ -13532,10 +13532,10 @@
         <v>1</v>
       </c>
       <c r="F182" t="n">
-        <v>443432</v>
+        <v>439147</v>
       </c>
       <c r="G182" t="s">
-        <v>79</v>
+        <v>364</v>
       </c>
       <c r="H182" t="s">
         <v>3</v>
@@ -13544,10 +13544,10 @@
         <v>1340245</v>
       </c>
       <c r="J182" t="s">
+        <v>362</v>
+      </c>
+      <c r="K182" t="s">
         <v>363</v>
-      </c>
-      <c r="K182" t="s">
-        <v>364</v>
       </c>
       <c r="L182" t="n">
         <v>0</v>
@@ -13620,10 +13620,10 @@
         <v>1340245</v>
       </c>
       <c r="J184" t="s">
+        <v>362</v>
+      </c>
+      <c r="K184" t="s">
         <v>363</v>
-      </c>
-      <c r="K184" t="s">
-        <v>364</v>
       </c>
       <c r="L184" t="n">
         <v>0</v>
@@ -13669,13 +13669,13 @@
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>12822</v>
+        <v>12825</v>
       </c>
       <c r="B186" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C186" t="s">
-        <v>362</v>
+        <v>78</v>
       </c>
       <c r="D186" t="n">
         <v>0</v>
@@ -13684,10 +13684,10 @@
         <v>1</v>
       </c>
       <c r="F186" t="n">
-        <v>439147</v>
+        <v>443432</v>
       </c>
       <c r="G186" t="s">
-        <v>362</v>
+        <v>79</v>
       </c>
       <c r="H186" t="s">
         <v>3</v>
@@ -13696,10 +13696,10 @@
         <v>1340245</v>
       </c>
       <c r="J186" t="s">
+        <v>362</v>
+      </c>
+      <c r="K186" t="s">
         <v>363</v>
-      </c>
-      <c r="K186" t="s">
-        <v>364</v>
       </c>
       <c r="L186" t="n">
         <v>0</v>
@@ -13745,13 +13745,13 @@
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>12825</v>
+        <v>12822</v>
       </c>
       <c r="B188" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C188" t="s">
-        <v>78</v>
+        <v>364</v>
       </c>
       <c r="D188" t="n">
         <v>0</v>
@@ -13760,10 +13760,10 @@
         <v>1</v>
       </c>
       <c r="F188" t="n">
-        <v>443432</v>
+        <v>439147</v>
       </c>
       <c r="G188" t="s">
-        <v>79</v>
+        <v>364</v>
       </c>
       <c r="H188" t="s">
         <v>3</v>
@@ -13772,10 +13772,10 @@
         <v>1340245</v>
       </c>
       <c r="J188" t="s">
+        <v>362</v>
+      </c>
+      <c r="K188" t="s">
         <v>363</v>
-      </c>
-      <c r="K188" t="s">
-        <v>364</v>
       </c>
       <c r="L188" t="n">
         <v>0</v>

</xml_diff>